<commit_message>
Fixed PB issues in DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBPB_ControlAppearance.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBPB_ControlAppearance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="211">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -860,29 +860,6 @@
 };</t>
   </si>
   <si>
-    <t>wait(2);
-validate1;
-link_Click(controlappearance_test_link);
-wait(2);
-validate2;
-SelectTestToRun(VT056_0464_string);
-validate3;
-ClickRunTest(runtest_top_xpath);
-SelectTestToRun(VT056_0521_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
-wait(2);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(BackButton_xpath);
-wait(10);
-TakeScreenshot(VT056_0521);
-validate5;
-ClickNativeIcon(ForwardButton_xpath);
-wait(10);
-SwitchApp(WEBVIEW);
-validate2;</t>
-  </si>
-  <si>
     <t>Note: Run this test with Javascript object.
 GoButton Visible</t>
   </si>
@@ -1950,21 +1927,6 @@
 BackButton Imageup(http)</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>wait(2);
-validate1;
-link_Click(controlappearance_test_link);
-wait(2);
-validate2;
-SelectTestToRun(VT056_0473_string);
-validate3;
-ClickRunTest(runtest_top_xpath);
-TakeScreenshot(VT056_0473);
-validate4;</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Pocket Browser Tests
@@ -2080,18 +2042,6 @@
 {
 validate_isIconDisplayed=ForwardButton_xpath,true
 };</t>
-  </si>
-  <si>
-    <t>wait(2);
-validate1;
-link_Click(controlappearance_test_link);
-wait(2);
-validate2;
-SelectTestToRun(VT056_0516_string);
-validate3;
-ClickRunTest(runtest_top_xpath);
-TakeScreenshot(VT056_0516);
-validate4;</t>
   </si>
   <si>
     <t>validate1
@@ -2315,6 +2265,60 @@
   </si>
   <si>
     <t>PB-Controls And Appearance</t>
+  </si>
+  <si>
+    <t>wait(2);
+validate1;
+link_Click(controlappearance_test_link);
+wait(2);
+validate2;
+SelectTestToRun(VT056_0473_string);
+validate3;
+ClickRunTest(runtest_top_xpath);
+wait(10);
+TakeScreenshot(VT056_0473);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(2);
+validate1;
+link_Click(controlappearance_test_link);
+wait(2);
+validate2;
+SelectTestToRun(VT056_0516_string);
+validate3;
+ClickRunTest(runtest_top_xpath);
+wait(10);
+TakeScreenshot(VT056_0516);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(2);
+validate1;
+link_Click(controlappearance_test_link);
+wait(2);
+validate2;
+SelectTestToRun(VT056_0464_string);
+validate3;
+ClickRunTest(runtest_top_xpath);
+wait(5);
+SelectTestToRun(VT056_0521_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+wait(2);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(BackButton_xpath);
+wait(5);
+TakeScreenshot(VT056_0521);
+validate5;
+link_Click(controlappearance_test_link);
+wait(5);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(BackButton_xpath);
+ClickNativeIcon(ForwardButton_xpath);
+wait(5);
+SwitchApp(WEBVIEW);
+validate2;</t>
   </si>
 </sst>
 </file>
@@ -2803,9 +2807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2859,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -3243,16 +3245,16 @@
         <v>10</v>
       </c>
       <c r="E16" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>180</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>183</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -3270,16 +3272,16 @@
         <v>10</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -3297,16 +3299,16 @@
         <v>10</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -3594,16 +3596,16 @@
         <v>10</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -3621,16 +3623,16 @@
         <v>10</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -3648,22 +3650,22 @@
         <v>10</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="268.5" thickBot="1">
+    <row r="32" spans="1:11" ht="332.25" thickBot="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3681,10 +3683,10 @@
         <v>1</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -3702,16 +3704,16 @@
         <v>10</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -3729,16 +3731,16 @@
         <v>10</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -3756,16 +3758,16 @@
         <v>10</v>
       </c>
       <c r="E35" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="G35" s="11" t="s">
+      <c r="H35" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>95</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -3783,16 +3785,16 @@
         <v>10</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -3810,16 +3812,16 @@
         <v>10</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="H37" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -3837,16 +3839,16 @@
         <v>10</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -3864,16 +3866,16 @@
         <v>10</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H39" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>107</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -3891,16 +3893,16 @@
         <v>10</v>
       </c>
       <c r="E40" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H40" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="F40" s="1">
-        <v>1</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -3918,16 +3920,16 @@
         <v>10</v>
       </c>
       <c r="E41" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="11" t="s">
+      <c r="H41" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>113</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -3945,16 +3947,16 @@
         <v>10</v>
       </c>
       <c r="E42" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="F42" s="1">
-        <v>1</v>
-      </c>
-      <c r="G42" s="11" t="s">
+      <c r="H42" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -3972,16 +3974,16 @@
         <v>10</v>
       </c>
       <c r="E43" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="F43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="11" t="s">
+      <c r="H43" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -3999,16 +4001,16 @@
         <v>10</v>
       </c>
       <c r="E44" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F44" s="1">
-        <v>1</v>
-      </c>
-      <c r="G44" s="11" t="s">
+      <c r="H44" s="11" t="s">
         <v>121</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>122</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -4026,16 +4028,16 @@
         <v>10</v>
       </c>
       <c r="E45" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-      <c r="G45" s="11" t="s">
+      <c r="H45" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -4053,16 +4055,16 @@
         <v>10</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -4080,16 +4082,16 @@
         <v>10</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -4107,16 +4109,16 @@
         <v>10</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F48" s="1">
         <v>1</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -4134,16 +4136,16 @@
         <v>10</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -4161,16 +4163,16 @@
         <v>10</v>
       </c>
       <c r="E50" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1</v>
+      </c>
+      <c r="G50" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="F50" s="1">
-        <v>1</v>
-      </c>
-      <c r="G50" s="11" t="s">
+      <c r="H50" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -4185,19 +4187,19 @@
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="1" t="s">
-        <v>181</v>
+        <v>10</v>
       </c>
       <c r="E51" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="H51" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="F51" s="1">
-        <v>1</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>146</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -4212,19 +4214,19 @@
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="1" t="s">
-        <v>181</v>
+        <v>10</v>
       </c>
       <c r="E52" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H52" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="F52" s="1">
-        <v>1</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>149</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -4242,16 +4244,16 @@
         <v>10</v>
       </c>
       <c r="E53" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="F53" s="1">
-        <v>1</v>
-      </c>
-      <c r="G53" s="11" t="s">
+      <c r="H53" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -4269,16 +4271,16 @@
         <v>10</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F54" s="1">
         <v>1</v>
       </c>
       <c r="G54" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H54" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>154</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -4296,16 +4298,16 @@
         <v>10</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -4323,16 +4325,16 @@
         <v>10</v>
       </c>
       <c r="E56" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="F56" s="1">
-        <v>1</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H56" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -4356,10 +4358,10 @@
         <v>1</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -4383,10 +4385,10 @@
         <v>1</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -4404,16 +4406,16 @@
         <v>10</v>
       </c>
       <c r="E59" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F59" s="1">
-        <v>1</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>163</v>
-      </c>
       <c r="H59" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -4431,16 +4433,16 @@
         <v>10</v>
       </c>
       <c r="E60" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="H60" s="11" t="s">
         <v>167</v>
-      </c>
-      <c r="F60" s="1">
-        <v>1</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>168</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -4455,19 +4457,19 @@
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="1" t="s">
-        <v>181</v>
+        <v>10</v>
       </c>
       <c r="E61" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="F61" s="1">
-        <v>1</v>
-      </c>
-      <c r="G61" s="11" t="s">
+      <c r="H61" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -4485,16 +4487,16 @@
         <v>10</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F62" s="1">
         <v>1</v>
       </c>
       <c r="G62" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="H62" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>173</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -4512,16 +4514,16 @@
         <v>10</v>
       </c>
       <c r="E63" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F63" s="1">
-        <v>1</v>
-      </c>
-      <c r="G63" s="11" t="s">
+      <c r="H63" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -4706,16 +4708,16 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
@@ -4737,16 +4739,16 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>11</v>
@@ -4768,16 +4770,16 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>11</v>
@@ -4799,16 +4801,16 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>11</v>
@@ -4830,16 +4832,16 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>11</v>
@@ -4861,16 +4863,16 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>11</v>

</xml_diff>